<commit_message>
Changed capitalization and ordered alphabetically neighborhoods
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_GoBack" localSheetId="0">English!$D$10</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -161,156 +161,6 @@
     <t>Karanganyar (OS)</t>
   </si>
   <si>
-    <t>BUMI</t>
-  </si>
-  <si>
-    <t>KARANGASEM</t>
-  </si>
-  <si>
-    <t>PAJANG</t>
-  </si>
-  <si>
-    <t>PUCANG SAWIT</t>
-  </si>
-  <si>
-    <t>JAGALAN</t>
-  </si>
-  <si>
-    <t>PURWODINIGRATAN</t>
-  </si>
-  <si>
-    <t>SEWU</t>
-  </si>
-  <si>
-    <t>GANDEKAN</t>
-  </si>
-  <si>
-    <t>SANGKRAH</t>
-  </si>
-  <si>
-    <t>PASAR KLIWON</t>
-  </si>
-  <si>
-    <t>KEDUNG LUMBU</t>
-  </si>
-  <si>
-    <t>SEMANGGI</t>
-  </si>
-  <si>
-    <t>JOYOSURAN</t>
-  </si>
-  <si>
-    <t>DANUKUSUMAN</t>
-  </si>
-  <si>
-    <t>JOYOTAKAN</t>
-  </si>
-  <si>
-    <t>BALUWARTI</t>
-  </si>
-  <si>
-    <t>GAJAHAN</t>
-  </si>
-  <si>
-    <t>JAYENGAN</t>
-  </si>
-  <si>
-    <t>KRATONAN</t>
-  </si>
-  <si>
-    <t>SERENGAN</t>
-  </si>
-  <si>
-    <t>TIPES</t>
-  </si>
-  <si>
-    <t>PANULARAN</t>
-  </si>
-  <si>
-    <t>KEMLAYAN</t>
-  </si>
-  <si>
-    <t>KAUMAN</t>
-  </si>
-  <si>
-    <t>KAMPUNG BARU</t>
-  </si>
-  <si>
-    <t>KEPRABON</t>
-  </si>
-  <si>
-    <t>TIMURAN</t>
-  </si>
-  <si>
-    <t>SRIWEDARI</t>
-  </si>
-  <si>
-    <t>PENUMPING</t>
-  </si>
-  <si>
-    <t>KETELAN</t>
-  </si>
-  <si>
-    <t>PUNGGAWAN</t>
-  </si>
-  <si>
-    <t>MANKUBUMEN</t>
-  </si>
-  <si>
-    <t>KESTALAN</t>
-  </si>
-  <si>
-    <t>SETABELAN</t>
-  </si>
-  <si>
-    <t>KEPATIHAN KULON</t>
-  </si>
-  <si>
-    <t>KEPATIHAN WETAN</t>
-  </si>
-  <si>
-    <t>TEGALHARJO</t>
-  </si>
-  <si>
-    <t>JEBRES</t>
-  </si>
-  <si>
-    <t>GILINGAN</t>
-  </si>
-  <si>
-    <t>SUMBER</t>
-  </si>
-  <si>
-    <t>MANAHAN</t>
-  </si>
-  <si>
-    <t>PURWOSARI</t>
-  </si>
-  <si>
-    <t>LAWEYAN</t>
-  </si>
-  <si>
-    <t>SONDAKAN</t>
-  </si>
-  <si>
-    <t>KERTEN</t>
-  </si>
-  <si>
-    <t>JAJAR</t>
-  </si>
-  <si>
-    <t>BANYUANYAR</t>
-  </si>
-  <si>
-    <t>KADIPIRO</t>
-  </si>
-  <si>
-    <t>NUSUKAN</t>
-  </si>
-  <si>
-    <t>MOJOSONGO</t>
-  </si>
-  <si>
     <t>0-10 mins</t>
   </si>
   <si>
@@ -638,9 +488,6 @@
     <t>Pengumpulan Data dengan Flocktracker : Pengguna Angkot</t>
   </si>
   <si>
-    <t>SUDIROPRAJAN</t>
-  </si>
-  <si>
     <t>Boyolali (OS)</t>
   </si>
   <si>
@@ -648,6 +495,159 @@
   </si>
   <si>
     <t>Tidak tentu</t>
+  </si>
+  <si>
+    <t>Baluwarti</t>
+  </si>
+  <si>
+    <t>Banyuanyar</t>
+  </si>
+  <si>
+    <t>Bumi</t>
+  </si>
+  <si>
+    <t>Danukusuman</t>
+  </si>
+  <si>
+    <t>Gajahan</t>
+  </si>
+  <si>
+    <t>Gandekan</t>
+  </si>
+  <si>
+    <t>Gilingan</t>
+  </si>
+  <si>
+    <t>Jagalan</t>
+  </si>
+  <si>
+    <t>Jajar</t>
+  </si>
+  <si>
+    <t>Jayengan</t>
+  </si>
+  <si>
+    <t>Jebres</t>
+  </si>
+  <si>
+    <t>Joyosuran</t>
+  </si>
+  <si>
+    <t>Joyotakan</t>
+  </si>
+  <si>
+    <t>Kadipiro</t>
+  </si>
+  <si>
+    <t>Kampung Baru</t>
+  </si>
+  <si>
+    <t>Karangasem</t>
+  </si>
+  <si>
+    <t>Kauman</t>
+  </si>
+  <si>
+    <t>Kedung Lumbu</t>
+  </si>
+  <si>
+    <t>Kemlayan</t>
+  </si>
+  <si>
+    <t>Kepatihan Kulon</t>
+  </si>
+  <si>
+    <t>Kepatihan Wetan</t>
+  </si>
+  <si>
+    <t>Keprabon</t>
+  </si>
+  <si>
+    <t>Kerten</t>
+  </si>
+  <si>
+    <t>Kestalan</t>
+  </si>
+  <si>
+    <t>Ketelan</t>
+  </si>
+  <si>
+    <t>Kratonan</t>
+  </si>
+  <si>
+    <t>Laweyan</t>
+  </si>
+  <si>
+    <t>Manahan</t>
+  </si>
+  <si>
+    <t>Mankubumen</t>
+  </si>
+  <si>
+    <t>Mojosongo</t>
+  </si>
+  <si>
+    <t>Nusukan</t>
+  </si>
+  <si>
+    <t>Pajang</t>
+  </si>
+  <si>
+    <t>Panularan</t>
+  </si>
+  <si>
+    <t>Pasar Kliwon</t>
+  </si>
+  <si>
+    <t>Penumping</t>
+  </si>
+  <si>
+    <t>Pucang Sawit</t>
+  </si>
+  <si>
+    <t>Punggawan</t>
+  </si>
+  <si>
+    <t>Purwodinigratan</t>
+  </si>
+  <si>
+    <t>Purwosari</t>
+  </si>
+  <si>
+    <t>Sangkrah</t>
+  </si>
+  <si>
+    <t>Semanggi</t>
+  </si>
+  <si>
+    <t>Serengan</t>
+  </si>
+  <si>
+    <t>Setabelan</t>
+  </si>
+  <si>
+    <t>Sewu</t>
+  </si>
+  <si>
+    <t>Sondakan</t>
+  </si>
+  <si>
+    <t>Sriwedari</t>
+  </si>
+  <si>
+    <t>Sudiroprajan</t>
+  </si>
+  <si>
+    <t>Sumber</t>
+  </si>
+  <si>
+    <t>Tegalharjo</t>
+  </si>
+  <si>
+    <t>Timuran</t>
+  </si>
+  <si>
+    <t>Tipes</t>
   </si>
 </sst>
 </file>
@@ -934,52 +934,57 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1270,39 +1275,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:G62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="20.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="20.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="23" style="1" customWidth="1"/>
     <col min="15" max="15" width="24" style="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="1"/>
+    <col min="16" max="16" width="28.42578125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="15">
+    <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="15">
+    <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="2:16" s="10" customFormat="1" ht="26">
+    <row r="4" spans="2:16" s="10" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
         <v>8</v>
       </c>
@@ -1316,16 +1321,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>2</v>
@@ -1346,49 +1351,49 @@
         <v>6</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" s="10" customFormat="1" ht="39">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" s="10" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="B5" s="30"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="23" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" s="10" customFormat="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="31"/>
       <c r="C6" s="11" t="s">
         <v>24</v>
@@ -1430,10 +1435,10 @@
         <v>36</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>19</v>
       </c>
@@ -1452,7 +1457,7 @@
       <c r="O7" s="6"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
@@ -1466,40 +1471,40 @@
         <v>21</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="P8" s="28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="7" t="s">
         <v>13</v>
@@ -1511,80 +1516,80 @@
         <v>22</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="P9" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="6"/>
       <c r="F10" s="25" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="P10" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="C11" s="7" t="s">
         <v>14</v>
@@ -1592,40 +1597,40 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="25" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="P11" s="28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -1633,40 +1638,40 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="25" t="s">
-        <v>61</v>
+        <v>160</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>61</v>
+        <v>160</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="P12" s="28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -1674,30 +1679,30 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="25" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="14" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
@@ -1705,30 +1710,30 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="25" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="14" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="L14" s="14"/>
       <c r="M14" s="14" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="8" t="s">
         <v>18</v>
@@ -1736,15 +1741,15 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="25" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="14" t="s">
-        <v>206</v>
+        <v>155</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -1753,16 +1758,16 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
       <c r="F16" s="25" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1774,16 +1779,16 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
       <c r="F17" s="25" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1795,16 +1800,16 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
       <c r="F18" s="25" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1816,16 +1821,16 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="2:16">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
       <c r="F19" s="25" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1837,16 +1842,16 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5"/>
       <c r="F20" s="25" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1858,16 +1863,16 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="2:16">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
       <c r="F21" s="25" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -1879,16 +1884,16 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="2:16">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="18"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
       <c r="F22" s="25" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -1900,16 +1905,16 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="2:16">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="18"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
       <c r="F23" s="25" t="s">
-        <v>46</v>
+        <v>171</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>46</v>
+        <v>171</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1921,16 +1926,16 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="18"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
       <c r="F24" s="25" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1942,16 +1947,16 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="2:16">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="18"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
       <c r="F25" s="25" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1963,16 +1968,16 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="2:16">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="18"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
       <c r="F26" s="25" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -1984,16 +1989,16 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="18"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
       <c r="F27" s="25" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -2005,16 +2010,16 @@
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="2:16">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="18"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
       <c r="F28" s="25" t="s">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -2026,16 +2031,16 @@
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
     </row>
-    <row r="29" spans="2:16">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="18"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="5"/>
       <c r="F29" s="25" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -2047,16 +2052,16 @@
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
       <c r="F30" s="25" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -2068,16 +2073,16 @@
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
     </row>
-    <row r="31" spans="2:16">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
       <c r="F31" s="25" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -2089,16 +2094,16 @@
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="2:16">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
       <c r="F32" s="25" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -2110,16 +2115,16 @@
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
     </row>
-    <row r="33" spans="2:16">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="18"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
       <c r="F33" s="25" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2131,16 +2136,16 @@
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="2:16">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="18"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
       <c r="F34" s="25" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="G34" s="25" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2152,16 +2157,16 @@
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
     </row>
-    <row r="35" spans="2:16">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="18"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="5"/>
       <c r="F35" s="25" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2173,16 +2178,16 @@
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
     </row>
-    <row r="36" spans="2:16">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="18"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
       <c r="F36" s="25" t="s">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2194,16 +2199,16 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="2:16">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="18"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="5"/>
       <c r="F37" s="25" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2215,16 +2220,16 @@
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="2:16">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="18"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
       <c r="F38" s="25" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="G38" s="25" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2236,16 +2241,16 @@
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
     </row>
-    <row r="39" spans="2:16">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="18"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="5"/>
       <c r="F39" s="25" t="s">
-        <v>47</v>
+        <v>185</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>47</v>
+        <v>185</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2257,16 +2262,16 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
     </row>
-    <row r="40" spans="2:16">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="18"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
       <c r="E40" s="5"/>
       <c r="F40" s="25" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -2278,16 +2283,16 @@
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
     </row>
-    <row r="41" spans="2:16">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="18"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="5"/>
       <c r="F41" s="25" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="G41" s="25" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -2299,16 +2304,16 @@
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
     </row>
-    <row r="42" spans="2:16">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="18"/>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
       <c r="F42" s="25" t="s">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="G42" s="25" t="s">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
@@ -2320,16 +2325,16 @@
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
     </row>
-    <row r="43" spans="2:16">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="18"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
       <c r="E43" s="5"/>
       <c r="F43" s="25" t="s">
-        <v>48</v>
+        <v>189</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>48</v>
+        <v>189</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
@@ -2341,16 +2346,16 @@
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
     </row>
-    <row r="44" spans="2:16">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="18"/>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="5"/>
       <c r="F44" s="25" t="s">
-        <v>75</v>
+        <v>190</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>75</v>
+        <v>190</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -2362,16 +2367,16 @@
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
     </row>
-    <row r="45" spans="2:16">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="18"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5"/>
       <c r="F45" s="25" t="s">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -2383,16 +2388,16 @@
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
     </row>
-    <row r="46" spans="2:16">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="18"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="25" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
@@ -2404,16 +2409,16 @@
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
     </row>
-    <row r="47" spans="2:16">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="18"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="25" t="s">
-        <v>53</v>
+        <v>193</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>53</v>
+        <v>193</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -2425,16 +2430,16 @@
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
     </row>
-    <row r="48" spans="2:16">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="18"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="25" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
@@ -2446,16 +2451,16 @@
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="18"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="25" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
@@ -2467,16 +2472,16 @@
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="18"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="25" t="s">
-        <v>78</v>
+        <v>196</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>78</v>
+        <v>196</v>
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
@@ -2488,16 +2493,16 @@
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
     </row>
-    <row r="51" spans="2:16">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="18"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="25" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -2509,16 +2514,16 @@
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="2:16">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="18"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="25" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="G52" s="25" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
@@ -2530,16 +2535,16 @@
       <c r="O52" s="6"/>
       <c r="P52" s="6"/>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="18"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="25" t="s">
-        <v>72</v>
+        <v>199</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>72</v>
+        <v>199</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
@@ -2551,16 +2556,16 @@
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
     </row>
-    <row r="54" spans="2:16">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="18"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G54" s="25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
@@ -2572,16 +2577,16 @@
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
     </row>
-    <row r="55" spans="2:16">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" s="18"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="F55" s="25" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="G55" s="25" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
@@ -2593,16 +2598,16 @@
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
     </row>
-    <row r="56" spans="2:16">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56" s="18"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="25" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="G56" s="25" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -2614,16 +2619,16 @@
       <c r="O56" s="6"/>
       <c r="P56" s="6"/>
     </row>
-    <row r="57" spans="2:16">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="18"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="25" t="s">
-        <v>71</v>
+        <v>203</v>
       </c>
       <c r="G57" s="25" t="s">
-        <v>71</v>
+        <v>203</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
@@ -2635,16 +2640,16 @@
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
     </row>
-    <row r="58" spans="2:16">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58" s="18"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
       <c r="F58" s="26" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
@@ -2656,16 +2661,16 @@
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
     </row>
-    <row r="59" spans="2:16">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59" s="18"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="24" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -2677,7 +2682,7 @@
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
     </row>
-    <row r="60" spans="2:16">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="18"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -2698,16 +2703,16 @@
       <c r="O60" s="6"/>
       <c r="P60" s="6"/>
     </row>
-    <row r="61" spans="2:16">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" s="18"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="F61" s="25" t="s">
-        <v>42</v>
+        <v>206</v>
       </c>
       <c r="G61" s="25" t="s">
-        <v>42</v>
+        <v>206</v>
       </c>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
@@ -2719,16 +2724,16 @@
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
     </row>
-    <row r="62" spans="2:16">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B62" s="19"/>
       <c r="C62" s="27"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6" t="s">
-        <v>43</v>
+        <v>207</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>43</v>
+        <v>207</v>
       </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
@@ -2740,11 +2745,11 @@
       <c r="O62" s="6"/>
       <c r="P62" s="6"/>
     </row>
-    <row r="63" spans="2:16">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C63" s="1"/>
       <c r="G63" s="16"/>
     </row>
-    <row r="68" spans="2:2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="15"/>
     </row>
   </sheetData>
@@ -2765,127 +2770,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P68"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:P6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="27.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
     <col min="13" max="13" width="23" style="1" customWidth="1"/>
-    <col min="14" max="15" width="27.1640625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="27.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="30" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="1"/>
+    <col min="17" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="15">
+    <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" ht="15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="2:16" s="10" customFormat="1" ht="26">
+    <row r="4" spans="2:16" s="10" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="O4" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>195</v>
-      </c>
       <c r="P4" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" s="10" customFormat="1" ht="52">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="B5" s="30"/>
       <c r="C5" s="21" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="23" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" s="10" customFormat="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="31"/>
       <c r="C6" s="11" t="s">
         <v>24</v>
@@ -2927,12 +2932,12 @@
         <v>36</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
@@ -2949,139 +2954,139 @@
       <c r="O7" s="6"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>21</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="P8" s="28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="P9" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="6"/>
       <c r="F10" s="25" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="P10" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="C11" s="7" t="s">
         <v>14</v>
@@ -3089,40 +3094,40 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="25" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="P11" s="28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -3130,40 +3135,40 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="25" t="s">
-        <v>61</v>
+        <v>160</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>61</v>
+        <v>160</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="P12" s="28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
@@ -3171,30 +3176,30 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="25" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>52</v>
+        <v>161</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="14" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="14"/>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
@@ -3202,30 +3207,30 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="25" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="14" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="L14" s="14"/>
       <c r="M14" s="14" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="18"/>
       <c r="C15" s="8" t="s">
         <v>18</v>
@@ -3233,15 +3238,15 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="25" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="14" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -3250,16 +3255,16 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="18"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
       <c r="F16" s="25" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -3271,16 +3276,16 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="2:16">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
       <c r="F17" s="25" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -3292,16 +3297,16 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="2:16">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="18"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
       <c r="F18" s="25" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>82</v>
+        <v>166</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -3313,16 +3318,16 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="2:16">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
       <c r="F19" s="25" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -3334,16 +3339,16 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="2:16">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5"/>
       <c r="F20" s="25" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>59</v>
+        <v>168</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -3355,16 +3360,16 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="2:16">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
       <c r="F21" s="25" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -3376,16 +3381,16 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="2:16">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="18"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
       <c r="F22" s="25" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -3397,16 +3402,16 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="2:16">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="18"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="5"/>
       <c r="F23" s="25" t="s">
-        <v>46</v>
+        <v>171</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>46</v>
+        <v>171</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -3418,16 +3423,16 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="18"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
       <c r="F24" s="25" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -3439,16 +3444,16 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="2:16">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="18"/>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5"/>
       <c r="F25" s="25" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>55</v>
+        <v>172</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -3460,16 +3465,16 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="2:16">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="18"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
       <c r="F26" s="25" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -3481,16 +3486,16 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="18"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
       <c r="F27" s="25" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -3502,16 +3507,16 @@
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="2:16">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="18"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
       <c r="F28" s="25" t="s">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -3523,16 +3528,16 @@
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
     </row>
-    <row r="29" spans="2:16">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="18"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="5"/>
       <c r="F29" s="25" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -3544,16 +3549,16 @@
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
       <c r="F30" s="25" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -3565,16 +3570,16 @@
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
     </row>
-    <row r="31" spans="2:16">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="18"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
       <c r="F31" s="25" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -3586,16 +3591,16 @@
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="2:16">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="18"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
       <c r="F32" s="25" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -3607,16 +3612,16 @@
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
     </row>
-    <row r="33" spans="2:16">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="18"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
       <c r="F33" s="25" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3628,16 +3633,16 @@
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="2:16">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="18"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="5"/>
       <c r="F34" s="25" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="G34" s="25" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3649,16 +3654,16 @@
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
     </row>
-    <row r="35" spans="2:16">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="18"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="5"/>
       <c r="F35" s="25" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3670,16 +3675,16 @@
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
     </row>
-    <row r="36" spans="2:16">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="18"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="5"/>
       <c r="F36" s="25" t="s">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3691,16 +3696,16 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="2:16">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="18"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
       <c r="E37" s="5"/>
       <c r="F37" s="25" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>94</v>
+        <v>183</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3712,16 +3717,16 @@
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="2:16">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="18"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
       <c r="E38" s="5"/>
       <c r="F38" s="25" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="G38" s="25" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3733,16 +3738,16 @@
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
     </row>
-    <row r="39" spans="2:16">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="18"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="5"/>
       <c r="F39" s="25" t="s">
-        <v>47</v>
+        <v>185</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>47</v>
+        <v>185</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3754,16 +3759,16 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
     </row>
-    <row r="40" spans="2:16">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="18"/>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
       <c r="E40" s="5"/>
       <c r="F40" s="25" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>66</v>
+        <v>186</v>
       </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -3775,16 +3780,16 @@
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
     </row>
-    <row r="41" spans="2:16">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="18"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
       <c r="E41" s="5"/>
       <c r="F41" s="25" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="G41" s="25" t="s">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -3796,16 +3801,16 @@
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
     </row>
-    <row r="42" spans="2:16">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="18"/>
       <c r="C42" s="5"/>
       <c r="D42" s="6"/>
       <c r="E42" s="5"/>
       <c r="F42" s="25" t="s">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="G42" s="25" t="s">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
@@ -3817,16 +3822,16 @@
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
     </row>
-    <row r="43" spans="2:16">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="18"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
       <c r="E43" s="5"/>
       <c r="F43" s="25" t="s">
-        <v>48</v>
+        <v>189</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>48</v>
+        <v>189</v>
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
@@ -3838,16 +3843,16 @@
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
     </row>
-    <row r="44" spans="2:16">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="18"/>
       <c r="C44" s="5"/>
       <c r="D44" s="6"/>
       <c r="E44" s="5"/>
       <c r="F44" s="25" t="s">
-        <v>75</v>
+        <v>190</v>
       </c>
       <c r="G44" s="25" t="s">
-        <v>75</v>
+        <v>190</v>
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -3859,16 +3864,16 @@
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
     </row>
-    <row r="45" spans="2:16">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="18"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="5"/>
       <c r="F45" s="25" t="s">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -3880,16 +3885,16 @@
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
     </row>
-    <row r="46" spans="2:16">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="18"/>
       <c r="C46" s="5"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="25" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
@@ -3901,16 +3906,16 @@
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
     </row>
-    <row r="47" spans="2:16">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="18"/>
       <c r="C47" s="5"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="25" t="s">
-        <v>53</v>
+        <v>193</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>53</v>
+        <v>193</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -3922,16 +3927,16 @@
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
     </row>
-    <row r="48" spans="2:16">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="18"/>
       <c r="C48" s="5"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="25" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>56</v>
+        <v>194</v>
       </c>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
@@ -3943,16 +3948,16 @@
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" s="18"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="25" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
@@ -3964,16 +3969,16 @@
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B50" s="18"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="25" t="s">
-        <v>78</v>
+        <v>196</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>78</v>
+        <v>196</v>
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
@@ -3985,16 +3990,16 @@
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
     </row>
-    <row r="51" spans="2:16">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="18"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="25" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -4006,16 +4011,16 @@
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="2:16">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="18"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="25" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="G52" s="25" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
@@ -4027,16 +4032,16 @@
       <c r="O52" s="6"/>
       <c r="P52" s="6"/>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="18"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="25" t="s">
-        <v>72</v>
+        <v>199</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>72</v>
+        <v>199</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
@@ -4048,16 +4053,16 @@
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
     </row>
-    <row r="54" spans="2:16">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="18"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G54" s="25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
@@ -4069,16 +4074,16 @@
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
     </row>
-    <row r="55" spans="2:16">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" s="18"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="F55" s="25" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="G55" s="25" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
@@ -4090,16 +4095,16 @@
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
     </row>
-    <row r="56" spans="2:16">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56" s="18"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="25" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="G56" s="25" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -4111,16 +4116,16 @@
       <c r="O56" s="6"/>
       <c r="P56" s="6"/>
     </row>
-    <row r="57" spans="2:16">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" s="18"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="25" t="s">
-        <v>71</v>
+        <v>203</v>
       </c>
       <c r="G57" s="25" t="s">
-        <v>71</v>
+        <v>203</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
@@ -4132,16 +4137,16 @@
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
     </row>
-    <row r="58" spans="2:16">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58" s="18"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
       <c r="F58" s="26" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
@@ -4153,16 +4158,16 @@
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
     </row>
-    <row r="59" spans="2:16">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B59" s="18"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="24" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -4174,7 +4179,7 @@
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
     </row>
-    <row r="60" spans="2:16">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B60" s="18"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -4195,16 +4200,16 @@
       <c r="O60" s="6"/>
       <c r="P60" s="6"/>
     </row>
-    <row r="61" spans="2:16">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" s="18"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="F61" s="25" t="s">
-        <v>42</v>
+        <v>206</v>
       </c>
       <c r="G61" s="25" t="s">
-        <v>42</v>
+        <v>206</v>
       </c>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
@@ -4216,16 +4221,16 @@
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
     </row>
-    <row r="62" spans="2:16">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B62" s="19"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6" t="s">
-        <v>43</v>
+        <v>207</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>43</v>
+        <v>207</v>
       </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
@@ -4237,12 +4242,12 @@
       <c r="O62" s="6"/>
       <c r="P62" s="6"/>
     </row>
-    <row r="63" spans="2:16">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="1"/>
       <c r="G63" s="16"/>
     </row>
-    <row r="68" spans="2:2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="15"/>
     </row>
   </sheetData>
@@ -4265,7 +4270,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>